<commit_message>
Edits to printing code in read_ipr_fwds
</commit_message>
<xml_diff>
--- a/PythonApplication1/ipr_read_data.xlsx
+++ b/PythonApplication1/ipr_read_data.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Johnny\Documents\UT_Law\2L Fall\Intellectual Property Tech Policy [Golden]\Final Paper\IPRAnalysis\IPRAnalysis\PythonApplication1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
   <si>
     <t>Trial Number(s)</t>
   </si>
@@ -112,9 +117,6 @@
   </si>
   <si>
     <t>IPR2015-01411</t>
-  </si>
-  <si>
-    <t>anuary4,2017</t>
   </si>
   <si>
     <t>7664971</t>
@@ -294,12 +296,15 @@
   <si>
     <t>0076-IPR2014-01006 FWD (Hyundai v Autoliv).pdf</t>
   </si>
+  <si>
+    <t>01/04/2017</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -361,12 +366,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -413,7 +429,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,9 +461,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,6 +513,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -654,24 +706,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="10" width="40.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="10" width="40.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -747,7 +801,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -785,15 +839,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
@@ -802,7 +856,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>
@@ -811,27 +865,27 @@
         <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -840,36 +894,36 @@
         <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
@@ -878,42 +932,45 @@
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:12" ht="220.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>18</v>
@@ -922,103 +979,103 @@
         <v>19</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:12" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:12" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
@@ -1027,7 +1084,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>18</v>
@@ -1036,16 +1093,16 @@
         <v>19</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="K10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>